<commit_message>
editing the harmonized model
</commit_message>
<xml_diff>
--- a/Papers/PROFILES'15 - HDL - Towards A Harmonized Dataset Model for Open Data Portals/tables/Harmonised Dataset Model.xlsx
+++ b/Papers/PROFILES'15 - HDL - Towards A Harmonized Dataset Model for Open Data Portals/tables/Harmonised Dataset Model.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="25703"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ahmadassaf/Google Drive/PhD TelecomParisTech - EURECOM - France 2012-2015/My PhD Documents/Papers/PROFILES'15 - HDL - Towards A Harmonized Dataset Model for Open Data Portals/tables/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="75" yWindow="465" windowWidth="38325" windowHeight="16440" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="19160" windowHeight="23540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -823,7 +828,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1242,69 +1247,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1314,6 +1256,69 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="54">
@@ -1711,32 +1716,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B29" sqref="B28:E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="16.875" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.83203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="47.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="48.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="55.125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="36.125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="47.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="48.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="55.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="36.1640625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1"/>
-    <col min="10" max="10" width="135.625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="23.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="135.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="10" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.6640625" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="24.375" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="24.33203125" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="16384" width="11" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>36</v>
       </c>
@@ -1779,21 +1784,21 @@
       <c r="O1" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="57" t="s">
+      <c r="P1" s="36" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="15.75">
-      <c r="A2" s="44" t="s">
+    <row r="2" spans="1:16" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="56" t="s">
         <v>79</v>
       </c>
-      <c r="B2" s="44"/>
-      <c r="C2" s="44"/>
-      <c r="D2" s="44"/>
-      <c r="E2" s="44"/>
-      <c r="F2" s="44"/>
-      <c r="G2" s="44"/>
-      <c r="H2" s="44"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
       <c r="J2" s="3" t="s">
         <v>115</v>
       </c>
@@ -1803,7 +1808,7 @@
       <c r="L2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="M2" s="56" t="s">
+      <c r="M2" s="35" t="s">
         <v>143</v>
       </c>
       <c r="N2" s="27" t="s">
@@ -1812,12 +1817,12 @@
       <c r="O2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P2" s="56" t="s">
+      <c r="P2" s="35" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="3" spans="1:16">
-      <c r="A3" s="45" t="s">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A3" s="57" t="s">
         <v>37</v>
       </c>
       <c r="B3" s="9" t="s">
@@ -1853,12 +1858,12 @@
       <c r="O3" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="P3" s="56" t="s">
+      <c r="P3" s="35" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:16">
-      <c r="A4" s="45"/>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A4" s="57"/>
       <c r="B4" s="9" t="s">
         <v>40</v>
       </c>
@@ -1891,8 +1896,8 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:16">
-      <c r="A5" s="45"/>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="57"/>
       <c r="B5" s="9" t="s">
         <v>41</v>
       </c>
@@ -1913,15 +1918,15 @@
       <c r="L5" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="M5" s="56" t="s">
+      <c r="M5" s="35" t="s">
         <v>231</v>
       </c>
-      <c r="P5" s="56" t="s">
+      <c r="P5" s="35" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="6" spans="1:16">
-      <c r="A6" s="45"/>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="57"/>
       <c r="B6" s="9" t="s">
         <v>42</v>
       </c>
@@ -1941,8 +1946,8 @@
       <c r="K6" s="27"/>
       <c r="L6" s="27"/>
     </row>
-    <row r="7" spans="1:16">
-      <c r="A7" s="45"/>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="57"/>
       <c r="B7" s="9" t="s">
         <v>20</v>
       </c>
@@ -1962,8 +1967,8 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:16">
-      <c r="A8" s="45"/>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="57"/>
       <c r="B8" s="9" t="s">
         <v>43</v>
       </c>
@@ -1977,8 +1982,8 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="45"/>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A9" s="57"/>
       <c r="B9" s="9" t="s">
         <v>45</v>
       </c>
@@ -2004,8 +2009,8 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="45"/>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A10" s="57"/>
       <c r="B10" s="9" t="s">
         <v>0</v>
       </c>
@@ -2031,8 +2036,8 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="45"/>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A11" s="57"/>
       <c r="B11" s="9" t="s">
         <v>67</v>
       </c>
@@ -2048,8 +2053,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="45"/>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A12" s="57"/>
       <c r="B12" s="9" t="s">
         <v>68</v>
       </c>
@@ -2063,8 +2068,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="45"/>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="57"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
       <c r="D13" s="11" t="s">
@@ -2082,8 +2087,8 @@
         <v>225</v>
       </c>
     </row>
-    <row r="14" spans="1:16">
-      <c r="A14" s="45"/>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="57"/>
       <c r="B14" s="9"/>
       <c r="C14" s="9"/>
       <c r="D14" s="11" t="s">
@@ -2103,8 +2108,8 @@
         <v>226</v>
       </c>
     </row>
-    <row r="15" spans="1:16">
-      <c r="A15" s="45"/>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="57"/>
       <c r="B15" s="9"/>
       <c r="C15" s="9"/>
       <c r="D15" s="11" t="s">
@@ -2122,8 +2127,8 @@
         <v>227</v>
       </c>
     </row>
-    <row r="16" spans="1:16">
-      <c r="A16" s="46" t="s">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="41" t="s">
         <v>52</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -2149,8 +2154,8 @@
         <v>228</v>
       </c>
     </row>
-    <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="42"/>
       <c r="B17" s="12" t="s">
         <v>54</v>
       </c>
@@ -2166,8 +2171,8 @@
         <v>229</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="42"/>
       <c r="B18" s="12" t="s">
         <v>55</v>
       </c>
@@ -2185,8 +2190,8 @@
         <v>230</v>
       </c>
     </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="47"/>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="42"/>
       <c r="B19" s="12" t="s">
         <v>44</v>
       </c>
@@ -2205,8 +2210,8 @@
       </c>
       <c r="H19" s="12"/>
     </row>
-    <row r="20" spans="1:10">
-      <c r="A20" s="47"/>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="42"/>
       <c r="B20" s="12"/>
       <c r="C20" s="12"/>
       <c r="D20" s="12" t="s">
@@ -2221,8 +2226,8 @@
       <c r="G20" s="12"/>
       <c r="H20" s="12"/>
     </row>
-    <row r="21" spans="1:10">
-      <c r="A21" s="47"/>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="42"/>
       <c r="B21" s="14" t="s">
         <v>119</v>
       </c>
@@ -2235,8 +2240,8 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="1:10">
-      <c r="A22" s="48"/>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="43"/>
       <c r="B22" s="14"/>
       <c r="C22" s="12"/>
       <c r="D22" s="12"/>
@@ -2247,8 +2252,8 @@
         <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:10">
-      <c r="A23" s="49" t="s">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="47" t="s">
         <v>61</v>
       </c>
       <c r="B23" s="8" t="s">
@@ -2263,8 +2268,8 @@
       </c>
       <c r="H23" s="8"/>
     </row>
-    <row r="24" spans="1:10">
-      <c r="A24" s="50"/>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="48"/>
       <c r="B24" s="8" t="s">
         <v>66</v>
       </c>
@@ -2275,8 +2280,8 @@
       <c r="G24" s="33"/>
       <c r="H24" s="8"/>
     </row>
-    <row r="25" spans="1:10">
-      <c r="A25" s="50"/>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A25" s="48"/>
       <c r="B25" s="8" t="s">
         <v>77</v>
       </c>
@@ -2295,8 +2300,8 @@
       </c>
       <c r="H25" s="8"/>
     </row>
-    <row r="26" spans="1:10">
-      <c r="A26" s="50"/>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="48"/>
       <c r="B26" s="8" t="s">
         <v>78</v>
       </c>
@@ -2317,8 +2322,8 @@
       </c>
       <c r="H26" s="8"/>
     </row>
-    <row r="27" spans="1:10">
-      <c r="A27" s="50"/>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="48"/>
       <c r="B27" s="8" t="s">
         <v>49</v>
       </c>
@@ -2331,8 +2336,8 @@
       <c r="G27" s="8"/>
       <c r="H27" s="8"/>
     </row>
-    <row r="28" spans="1:10">
-      <c r="A28" s="50"/>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="48"/>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
       <c r="D28" s="8" t="s">
@@ -2349,8 +2354,8 @@
       </c>
       <c r="H28" s="8"/>
     </row>
-    <row r="29" spans="1:10">
-      <c r="A29" s="51"/>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="58"/>
       <c r="B29" s="8"/>
       <c r="C29" s="8"/>
       <c r="D29" s="8" t="s">
@@ -2367,8 +2372,8 @@
       </c>
       <c r="H29" s="8"/>
     </row>
-    <row r="30" spans="1:10">
-      <c r="A30" s="37" t="s">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="49" t="s">
         <v>80</v>
       </c>
       <c r="B30" s="15" t="s">
@@ -2391,8 +2396,8 @@
         <v>128</v>
       </c>
     </row>
-    <row r="31" spans="1:10">
-      <c r="A31" s="38"/>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="50"/>
       <c r="B31" s="15" t="s">
         <v>35</v>
       </c>
@@ -2402,7 +2407,7 @@
       <c r="D31" s="28" t="s">
         <v>139</v>
       </c>
-      <c r="E31" s="55" t="s">
+      <c r="E31" s="34" t="s">
         <v>234</v>
       </c>
       <c r="F31" s="15"/>
@@ -2411,8 +2416,8 @@
       </c>
       <c r="H31" s="15"/>
     </row>
-    <row r="32" spans="1:10">
-      <c r="A32" s="38"/>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="50"/>
       <c r="B32" s="15" t="s">
         <v>81</v>
       </c>
@@ -2425,17 +2430,17 @@
       </c>
       <c r="H32" s="15"/>
     </row>
-    <row r="33" spans="1:8">
-      <c r="A33" s="38"/>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A33" s="50"/>
       <c r="B33" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C33" s="15"/>
       <c r="D33" s="15"/>
-      <c r="E33" s="55" t="s">
+      <c r="E33" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="F33" s="55" t="s">
+      <c r="F33" s="34" t="s">
         <v>210</v>
       </c>
       <c r="G33" s="28" t="s">
@@ -2443,8 +2448,8 @@
       </c>
       <c r="H33" s="15"/>
     </row>
-    <row r="34" spans="1:8">
-      <c r="A34" s="38"/>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A34" s="50"/>
       <c r="B34" s="15" t="s">
         <v>83</v>
       </c>
@@ -2463,8 +2468,8 @@
       </c>
       <c r="H34" s="15"/>
     </row>
-    <row r="35" spans="1:8">
-      <c r="A35" s="38"/>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A35" s="50"/>
       <c r="B35" s="15"/>
       <c r="C35" s="15"/>
       <c r="D35" s="15" t="s">
@@ -2475,8 +2480,8 @@
       <c r="G35" s="15"/>
       <c r="H35" s="15"/>
     </row>
-    <row r="36" spans="1:8">
-      <c r="A36" s="38"/>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A36" s="50"/>
       <c r="B36" s="15"/>
       <c r="C36" s="15"/>
       <c r="D36" s="15" t="s">
@@ -2487,8 +2492,8 @@
       <c r="G36" s="15"/>
       <c r="H36" s="15"/>
     </row>
-    <row r="37" spans="1:8">
-      <c r="A37" s="38"/>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A37" s="50"/>
       <c r="B37" s="15" t="s">
         <v>1</v>
       </c>
@@ -2501,8 +2506,8 @@
       </c>
       <c r="H37" s="15"/>
     </row>
-    <row r="38" spans="1:8" ht="15.75">
-      <c r="A38" s="38"/>
+    <row r="38" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" s="50"/>
       <c r="B38" s="16"/>
       <c r="C38" s="16"/>
       <c r="D38" s="16" t="s">
@@ -2515,8 +2520,8 @@
       </c>
       <c r="H38" s="16"/>
     </row>
-    <row r="39" spans="1:8" ht="15.75">
-      <c r="A39" s="38"/>
+    <row r="39" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A39" s="50"/>
       <c r="B39" s="16"/>
       <c r="C39" s="16"/>
       <c r="D39" s="16"/>
@@ -2527,8 +2532,8 @@
       </c>
       <c r="H39" s="16"/>
     </row>
-    <row r="40" spans="1:8" ht="15.75">
-      <c r="A40" s="38"/>
+    <row r="40" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A40" s="50"/>
       <c r="B40" s="16"/>
       <c r="C40" s="16"/>
       <c r="D40" s="16" t="s">
@@ -2539,8 +2544,8 @@
       <c r="G40" s="16"/>
       <c r="H40" s="16"/>
     </row>
-    <row r="41" spans="1:8" ht="15.75">
-      <c r="A41" s="38"/>
+    <row r="41" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="50"/>
       <c r="B41" s="16"/>
       <c r="C41" s="16"/>
       <c r="D41" s="16" t="s">
@@ -2551,8 +2556,8 @@
       <c r="G41" s="16"/>
       <c r="H41" s="16"/>
     </row>
-    <row r="42" spans="1:8" ht="15.75">
-      <c r="A42" s="38"/>
+    <row r="42" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A42" s="50"/>
       <c r="B42" s="16"/>
       <c r="C42" s="16"/>
       <c r="D42" s="16" t="s">
@@ -2563,8 +2568,8 @@
       <c r="G42" s="16"/>
       <c r="H42" s="16"/>
     </row>
-    <row r="43" spans="1:8" ht="15.75">
-      <c r="A43" s="39"/>
+    <row r="43" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+      <c r="A43" s="51"/>
       <c r="B43" s="16"/>
       <c r="C43" s="16"/>
       <c r="D43" s="16" t="s">
@@ -2575,8 +2580,8 @@
       <c r="G43" s="16"/>
       <c r="H43" s="16"/>
     </row>
-    <row r="44" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A44" s="40" t="s">
+    <row r="44" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="52" t="s">
         <v>131</v>
       </c>
       <c r="B44" s="20" t="s">
@@ -2597,8 +2602,8 @@
       </c>
       <c r="H44" s="21"/>
     </row>
-    <row r="45" spans="1:8">
-      <c r="A45" s="40"/>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" s="52"/>
       <c r="B45" s="20" t="s">
         <v>121</v>
       </c>
@@ -2609,8 +2614,8 @@
       <c r="G45" s="21"/>
       <c r="H45" s="21"/>
     </row>
-    <row r="46" spans="1:8">
-      <c r="A46" s="40"/>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" s="52"/>
       <c r="B46" s="20"/>
       <c r="C46" s="21"/>
       <c r="D46" s="21"/>
@@ -2621,8 +2626,8 @@
         <v>132</v>
       </c>
     </row>
-    <row r="47" spans="1:8">
-      <c r="A47" s="40"/>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" s="52"/>
       <c r="B47" s="20"/>
       <c r="C47" s="21"/>
       <c r="D47" s="21"/>
@@ -2633,8 +2638,8 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:8">
-      <c r="A48" s="40"/>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A48" s="52"/>
       <c r="B48" s="20"/>
       <c r="C48" s="21"/>
       <c r="D48" s="21"/>
@@ -2645,8 +2650,8 @@
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:8">
-      <c r="A49" s="40"/>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" s="52"/>
       <c r="B49" s="20"/>
       <c r="C49" s="21"/>
       <c r="D49" s="21"/>
@@ -2657,8 +2662,8 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A50" s="41" t="s">
+    <row r="50" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="53" t="s">
         <v>130</v>
       </c>
       <c r="B50" s="17"/>
@@ -2677,8 +2682,8 @@
       </c>
       <c r="H50" s="17"/>
     </row>
-    <row r="51" spans="1:8">
-      <c r="A51" s="42"/>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A51" s="54"/>
       <c r="B51" s="19" t="s">
         <v>117</v>
       </c>
@@ -2689,8 +2694,8 @@
       <c r="G51" s="18"/>
       <c r="H51" s="17"/>
     </row>
-    <row r="52" spans="1:8">
-      <c r="A52" s="42"/>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A52" s="54"/>
       <c r="B52" s="19" t="s">
         <v>116</v>
       </c>
@@ -2701,8 +2706,8 @@
       <c r="G52" s="18"/>
       <c r="H52" s="17"/>
     </row>
-    <row r="53" spans="1:8">
-      <c r="A53" s="43"/>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A53" s="55"/>
       <c r="B53" s="19" t="s">
         <v>118</v>
       </c>
@@ -2713,7 +2718,7 @@
       <c r="G53" s="18"/>
       <c r="H53" s="17"/>
     </row>
-    <row r="54" spans="1:8">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A54" s="23" t="s">
         <v>136</v>
       </c>
@@ -2731,20 +2736,20 @@
       </c>
       <c r="H54" s="25"/>
     </row>
-    <row r="55" spans="1:8">
-      <c r="A55" s="34" t="s">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A55" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B55" s="35"/>
-      <c r="C55" s="35"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="35"/>
-      <c r="G55" s="35"/>
-      <c r="H55" s="36"/>
-    </row>
-    <row r="56" spans="1:8">
-      <c r="A56" s="52" t="s">
+      <c r="B55" s="39"/>
+      <c r="C55" s="39"/>
+      <c r="D55" s="39"/>
+      <c r="E55" s="39"/>
+      <c r="F55" s="39"/>
+      <c r="G55" s="39"/>
+      <c r="H55" s="40"/>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A56" s="44" t="s">
         <v>37</v>
       </c>
       <c r="B56" s="9" t="s">
@@ -2765,8 +2770,8 @@
       </c>
       <c r="H56" s="9"/>
     </row>
-    <row r="57" spans="1:8">
-      <c r="A57" s="53"/>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A57" s="45"/>
       <c r="B57" s="9" t="s">
         <v>1</v>
       </c>
@@ -2779,8 +2784,8 @@
       </c>
       <c r="H57" s="9"/>
     </row>
-    <row r="58" spans="1:8">
-      <c r="A58" s="53"/>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A58" s="45"/>
       <c r="B58" s="9" t="s">
         <v>18</v>
       </c>
@@ -2791,8 +2796,8 @@
       <c r="G58" s="9"/>
       <c r="H58" s="9"/>
     </row>
-    <row r="59" spans="1:8">
-      <c r="A59" s="53"/>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A59" s="45"/>
       <c r="B59" s="9" t="s">
         <v>42</v>
       </c>
@@ -2805,8 +2810,8 @@
       </c>
       <c r="H59" s="9"/>
     </row>
-    <row r="60" spans="1:8">
-      <c r="A60" s="53"/>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A60" s="45"/>
       <c r="B60" s="9" t="s">
         <v>20</v>
       </c>
@@ -2819,8 +2824,8 @@
       </c>
       <c r="H60" s="9"/>
     </row>
-    <row r="61" spans="1:8">
-      <c r="A61" s="53"/>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A61" s="45"/>
       <c r="B61" s="9" t="s">
         <v>85</v>
       </c>
@@ -2831,8 +2836,8 @@
       <c r="G61" s="9"/>
       <c r="H61" s="9"/>
     </row>
-    <row r="62" spans="1:8">
-      <c r="A62" s="53"/>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A62" s="45"/>
       <c r="B62" s="9" t="s">
         <v>41</v>
       </c>
@@ -2843,8 +2848,8 @@
       <c r="G62" s="9"/>
       <c r="H62" s="9"/>
     </row>
-    <row r="63" spans="1:8">
-      <c r="A63" s="53"/>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A63" s="45"/>
       <c r="B63" s="9" t="s">
         <v>86</v>
       </c>
@@ -2855,8 +2860,8 @@
       <c r="G63" s="9"/>
       <c r="H63" s="9"/>
     </row>
-    <row r="64" spans="1:8">
-      <c r="A64" s="53"/>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A64" s="45"/>
       <c r="B64" s="9" t="s">
         <v>87</v>
       </c>
@@ -2867,8 +2872,8 @@
       <c r="G64" s="9"/>
       <c r="H64" s="9"/>
     </row>
-    <row r="65" spans="1:8">
-      <c r="A65" s="54"/>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A65" s="46"/>
       <c r="B65" s="9"/>
       <c r="C65" s="9"/>
       <c r="D65" s="9" t="s">
@@ -2881,8 +2886,8 @@
       </c>
       <c r="H65" s="9"/>
     </row>
-    <row r="66" spans="1:8">
-      <c r="A66" s="49" t="s">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A66" s="47" t="s">
         <v>61</v>
       </c>
       <c r="B66" s="8" t="s">
@@ -2895,8 +2900,8 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8"/>
     </row>
-    <row r="67" spans="1:8">
-      <c r="A67" s="51"/>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A67" s="58"/>
       <c r="B67" s="8" t="s">
         <v>66</v>
       </c>
@@ -2907,20 +2912,20 @@
       <c r="G67" s="8"/>
       <c r="H67" s="8"/>
     </row>
-    <row r="68" spans="1:8">
-      <c r="A68" s="34" t="s">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A68" s="38" t="s">
         <v>9</v>
       </c>
-      <c r="B68" s="35"/>
-      <c r="C68" s="35"/>
-      <c r="D68" s="35"/>
-      <c r="E68" s="35"/>
-      <c r="F68" s="35"/>
-      <c r="G68" s="35"/>
-      <c r="H68" s="36"/>
-    </row>
-    <row r="69" spans="1:8">
-      <c r="A69" s="52" t="s">
+      <c r="B68" s="39"/>
+      <c r="C68" s="39"/>
+      <c r="D68" s="39"/>
+      <c r="E68" s="39"/>
+      <c r="F68" s="39"/>
+      <c r="G68" s="39"/>
+      <c r="H68" s="40"/>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A69" s="44" t="s">
         <v>56</v>
       </c>
       <c r="B69" s="9" t="s">
@@ -2935,8 +2940,8 @@
       <c r="G69" s="9"/>
       <c r="H69" s="9"/>
     </row>
-    <row r="70" spans="1:8">
-      <c r="A70" s="53"/>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A70" s="45"/>
       <c r="B70" s="9" t="s">
         <v>18</v>
       </c>
@@ -2951,8 +2956,8 @@
         <v>126</v>
       </c>
     </row>
-    <row r="71" spans="1:8">
-      <c r="A71" s="53"/>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A71" s="45"/>
       <c r="B71" s="9" t="s">
         <v>58</v>
       </c>
@@ -2969,8 +2974,8 @@
       </c>
       <c r="H71" s="9"/>
     </row>
-    <row r="72" spans="1:8">
-      <c r="A72" s="53"/>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A72" s="45"/>
       <c r="B72" s="9" t="s">
         <v>41</v>
       </c>
@@ -2983,8 +2988,8 @@
       <c r="G72" s="9"/>
       <c r="H72" s="9"/>
     </row>
-    <row r="73" spans="1:8">
-      <c r="A73" s="53"/>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A73" s="45"/>
       <c r="B73" s="9" t="s">
         <v>59</v>
       </c>
@@ -2995,8 +3000,8 @@
       <c r="G73" s="9"/>
       <c r="H73" s="9"/>
     </row>
-    <row r="74" spans="1:8">
-      <c r="A74" s="53"/>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A74" s="45"/>
       <c r="B74" s="9" t="s">
         <v>1</v>
       </c>
@@ -3015,8 +3020,8 @@
       </c>
       <c r="H74" s="9"/>
     </row>
-    <row r="75" spans="1:8">
-      <c r="A75" s="53"/>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A75" s="45"/>
       <c r="B75" s="9" t="s">
         <v>60</v>
       </c>
@@ -3037,8 +3042,8 @@
       </c>
       <c r="H75" s="9"/>
     </row>
-    <row r="76" spans="1:8">
-      <c r="A76" s="53"/>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A76" s="45"/>
       <c r="B76" s="10" t="s">
         <v>71</v>
       </c>
@@ -3055,8 +3060,8 @@
       <c r="G76" s="9"/>
       <c r="H76" s="9"/>
     </row>
-    <row r="77" spans="1:8">
-      <c r="A77" s="53"/>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A77" s="45"/>
       <c r="B77" s="9" t="s">
         <v>69</v>
       </c>
@@ -3067,8 +3072,8 @@
       <c r="G77" s="9"/>
       <c r="H77" s="9"/>
     </row>
-    <row r="78" spans="1:8">
-      <c r="A78" s="53"/>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A78" s="45"/>
       <c r="B78" s="9" t="s">
         <v>20</v>
       </c>
@@ -3089,8 +3094,8 @@
         <v>127</v>
       </c>
     </row>
-    <row r="79" spans="1:8">
-      <c r="A79" s="53"/>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A79" s="45"/>
       <c r="B79" s="9" t="s">
         <v>74</v>
       </c>
@@ -3101,8 +3106,8 @@
       <c r="G79" s="9"/>
       <c r="H79" s="9"/>
     </row>
-    <row r="80" spans="1:8">
-      <c r="A80" s="53"/>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A80" s="45"/>
       <c r="B80" s="9" t="s">
         <v>75</v>
       </c>
@@ -3115,8 +3120,8 @@
       </c>
       <c r="H80" s="9"/>
     </row>
-    <row r="81" spans="1:8">
-      <c r="A81" s="53"/>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A81" s="45"/>
       <c r="B81" s="9"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9" t="s">
@@ -3127,8 +3132,8 @@
       <c r="G81" s="9"/>
       <c r="H81" s="9"/>
     </row>
-    <row r="82" spans="1:8">
-      <c r="A82" s="53"/>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A82" s="45"/>
       <c r="B82" s="9"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9" t="s">
@@ -3139,8 +3144,8 @@
       <c r="G82" s="9"/>
       <c r="H82" s="9"/>
     </row>
-    <row r="83" spans="1:8">
-      <c r="A83" s="54"/>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A83" s="46"/>
       <c r="B83" s="9"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9" t="s">
@@ -3151,8 +3156,8 @@
       <c r="G83" s="9"/>
       <c r="H83" s="9"/>
     </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="46" t="s">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A84" s="41" t="s">
         <v>52</v>
       </c>
       <c r="B84" s="12" t="s">
@@ -3165,8 +3170,8 @@
       <c r="G84" s="12"/>
       <c r="H84" s="12"/>
     </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="47"/>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A85" s="42"/>
       <c r="B85" s="12" t="s">
         <v>70</v>
       </c>
@@ -3177,8 +3182,8 @@
       <c r="G85" s="12"/>
       <c r="H85" s="12"/>
     </row>
-    <row r="86" spans="1:8">
-      <c r="A86" s="47"/>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A86" s="42"/>
       <c r="B86" s="12" t="s">
         <v>44</v>
       </c>
@@ -3191,7 +3196,7 @@
       <c r="E86" s="30" t="s">
         <v>162</v>
       </c>
-      <c r="F86" s="58" t="s">
+      <c r="F86" s="37" t="s">
         <v>207</v>
       </c>
       <c r="G86" s="30" t="s">
@@ -3199,8 +3204,8 @@
       </c>
       <c r="H86" s="12"/>
     </row>
-    <row r="87" spans="1:8">
-      <c r="A87" s="47"/>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A87" s="42"/>
       <c r="B87" s="12"/>
       <c r="C87" s="12"/>
       <c r="D87" s="12" t="s">
@@ -3217,8 +3222,8 @@
         <v>31</v>
       </c>
     </row>
-    <row r="88" spans="1:8">
-      <c r="A88" s="48"/>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A88" s="43"/>
       <c r="B88" s="12" t="s">
         <v>73</v>
       </c>
@@ -3229,8 +3234,8 @@
       <c r="G88" s="12"/>
       <c r="H88" s="12"/>
     </row>
-    <row r="89" spans="1:8">
-      <c r="A89" s="49" t="s">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A89" s="47" t="s">
         <v>61</v>
       </c>
       <c r="B89" s="8" t="s">
@@ -3243,8 +3248,8 @@
       <c r="G89" s="33"/>
       <c r="H89" s="8"/>
     </row>
-    <row r="90" spans="1:8">
-      <c r="A90" s="50"/>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A90" s="48"/>
       <c r="B90" s="8" t="s">
         <v>49</v>
       </c>
@@ -3257,8 +3262,8 @@
       <c r="G90" s="8"/>
       <c r="H90" s="8"/>
     </row>
-    <row r="91" spans="1:8">
-      <c r="A91" s="50"/>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A91" s="48"/>
       <c r="B91" s="8" t="s">
         <v>63</v>
       </c>
@@ -3269,8 +3274,8 @@
       <c r="G91" s="8"/>
       <c r="H91" s="8"/>
     </row>
-    <row r="92" spans="1:8">
-      <c r="A92" s="50"/>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A92" s="48"/>
       <c r="B92" s="8" t="s">
         <v>64</v>
       </c>
@@ -3287,8 +3292,8 @@
         <v>25</v>
       </c>
     </row>
-    <row r="93" spans="1:8">
-      <c r="A93" s="50"/>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A93" s="48"/>
       <c r="B93" s="8" t="s">
         <v>65</v>
       </c>
@@ -3305,8 +3310,8 @@
         <v>26</v>
       </c>
     </row>
-    <row r="94" spans="1:8">
-      <c r="A94" s="50"/>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A94" s="48"/>
       <c r="B94" s="8" t="s">
         <v>66</v>
       </c>
@@ -3319,20 +3324,20 @@
       <c r="G94" s="8"/>
       <c r="H94" s="8"/>
     </row>
-    <row r="95" spans="1:8">
-      <c r="A95" s="34" t="s">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A95" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="B95" s="35"/>
-      <c r="C95" s="35"/>
-      <c r="D95" s="35"/>
-      <c r="E95" s="35"/>
-      <c r="F95" s="35"/>
-      <c r="G95" s="35"/>
-      <c r="H95" s="36"/>
-    </row>
-    <row r="96" spans="1:8">
-      <c r="A96" s="46" t="s">
+      <c r="B95" s="39"/>
+      <c r="C95" s="39"/>
+      <c r="D95" s="39"/>
+      <c r="E95" s="39"/>
+      <c r="F95" s="39"/>
+      <c r="G95" s="39"/>
+      <c r="H95" s="40"/>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A96" s="41" t="s">
         <v>50</v>
       </c>
       <c r="B96" s="12" t="s">
@@ -3347,8 +3352,8 @@
       <c r="G96" s="12"/>
       <c r="H96" s="12"/>
     </row>
-    <row r="97" spans="1:8">
-      <c r="A97" s="47"/>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A97" s="42"/>
       <c r="B97" s="12" t="s">
         <v>1</v>
       </c>
@@ -3361,8 +3366,8 @@
       <c r="G97" s="12"/>
       <c r="H97" s="12"/>
     </row>
-    <row r="98" spans="1:8">
-      <c r="A98" s="47"/>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A98" s="42"/>
       <c r="B98" s="12" t="s">
         <v>0</v>
       </c>
@@ -3375,8 +3380,8 @@
       <c r="G98" s="12"/>
       <c r="H98" s="12"/>
     </row>
-    <row r="99" spans="1:8">
-      <c r="A99" s="47"/>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A99" s="42"/>
       <c r="B99" s="12" t="s">
         <v>47</v>
       </c>
@@ -3389,8 +3394,8 @@
       <c r="G99" s="12"/>
       <c r="H99" s="12"/>
     </row>
-    <row r="100" spans="1:8">
-      <c r="A100" s="47"/>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A100" s="42"/>
       <c r="B100" s="12" t="s">
         <v>18</v>
       </c>
@@ -3403,8 +3408,8 @@
       <c r="G100" s="12"/>
       <c r="H100" s="12"/>
     </row>
-    <row r="101" spans="1:8">
-      <c r="A101" s="47"/>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A101" s="42"/>
       <c r="B101" s="12" t="s">
         <v>20</v>
       </c>
@@ -3417,8 +3422,8 @@
       <c r="G101" s="12"/>
       <c r="H101" s="12"/>
     </row>
-    <row r="102" spans="1:8">
-      <c r="A102" s="48"/>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A102" s="43"/>
       <c r="B102" s="14" t="s">
         <v>122</v>
       </c>
@@ -3429,20 +3434,20 @@
       <c r="G102" s="12"/>
       <c r="H102" s="12"/>
     </row>
-    <row r="103" spans="1:8">
-      <c r="A103" s="34" t="s">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A103" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B103" s="35"/>
-      <c r="C103" s="35"/>
-      <c r="D103" s="35"/>
-      <c r="E103" s="35"/>
-      <c r="F103" s="35"/>
-      <c r="G103" s="35"/>
-      <c r="H103" s="36"/>
-    </row>
-    <row r="104" spans="1:8">
-      <c r="A104" s="46" t="s">
+      <c r="B103" s="39"/>
+      <c r="C103" s="39"/>
+      <c r="D103" s="39"/>
+      <c r="E103" s="39"/>
+      <c r="F103" s="39"/>
+      <c r="G103" s="39"/>
+      <c r="H103" s="40"/>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A104" s="41" t="s">
         <v>50</v>
       </c>
       <c r="B104" s="12" t="s">
@@ -3459,8 +3464,8 @@
       <c r="G104" s="12"/>
       <c r="H104" s="12"/>
     </row>
-    <row r="105" spans="1:8">
-      <c r="A105" s="47"/>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A105" s="42"/>
       <c r="B105" s="12" t="s">
         <v>46</v>
       </c>
@@ -3473,8 +3478,8 @@
       <c r="G105" s="12"/>
       <c r="H105" s="12"/>
     </row>
-    <row r="106" spans="1:8">
-      <c r="A106" s="47"/>
+    <row r="106" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A106" s="42"/>
       <c r="B106" s="12" t="s">
         <v>20</v>
       </c>
@@ -3489,8 +3494,8 @@
       <c r="G106" s="12"/>
       <c r="H106" s="12"/>
     </row>
-    <row r="107" spans="1:8">
-      <c r="A107" s="47"/>
+    <row r="107" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A107" s="42"/>
       <c r="B107" s="12" t="s">
         <v>41</v>
       </c>
@@ -3501,8 +3506,8 @@
       <c r="G107" s="12"/>
       <c r="H107" s="12"/>
     </row>
-    <row r="108" spans="1:8">
-      <c r="A108" s="48"/>
+    <row r="108" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A108" s="43"/>
       <c r="B108" s="12" t="s">
         <v>18</v>
       </c>
@@ -3515,7 +3520,7 @@
       <c r="G108" s="12"/>
       <c r="H108" s="12"/>
     </row>
-    <row r="109" spans="1:8">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A109" s="7" t="s">
         <v>51</v>
       </c>
@@ -3531,13 +3536,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A103:H103"/>
-    <mergeCell ref="A104:A108"/>
-    <mergeCell ref="A69:A83"/>
-    <mergeCell ref="A84:A88"/>
-    <mergeCell ref="A89:A94"/>
-    <mergeCell ref="A95:H95"/>
-    <mergeCell ref="A96:A102"/>
     <mergeCell ref="A68:H68"/>
     <mergeCell ref="A30:A43"/>
     <mergeCell ref="A44:A49"/>
@@ -3549,6 +3547,13 @@
     <mergeCell ref="A55:H55"/>
     <mergeCell ref="A56:A65"/>
     <mergeCell ref="A66:A67"/>
+    <mergeCell ref="A103:H103"/>
+    <mergeCell ref="A104:A108"/>
+    <mergeCell ref="A69:A83"/>
+    <mergeCell ref="A84:A88"/>
+    <mergeCell ref="A89:A94"/>
+    <mergeCell ref="A95:H95"/>
+    <mergeCell ref="A96:A102"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>

</xml_diff>